<commit_message>
added March and July methods comparisons
</commit_message>
<xml_diff>
--- a/week1/experiments/exp1/Kai_exp_1.xlsx
+++ b/week1/experiments/exp1/Kai_exp_1.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="16380" windowHeight="8190" tabRatio="993" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="16380" windowHeight="8190" tabRatio="484" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="23">
   <si>
     <t>Time</t>
   </si>
@@ -72,6 +72,18 @@
   </si>
   <si>
     <t>rate uM/H</t>
+  </si>
+  <si>
+    <t>using all data</t>
+  </si>
+  <si>
+    <t>Low_Water_Line</t>
+  </si>
+  <si>
+    <t>Seep</t>
+  </si>
+  <si>
+    <t>omit first 3 points</t>
   </si>
 </sst>
 </file>
@@ -1036,11 +1048,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="118957184"/>
-        <c:axId val="118958720"/>
+        <c:axId val="119612544"/>
+        <c:axId val="119614080"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="118957184"/>
+        <c:axId val="119612544"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1050,12 +1062,12 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="118958720"/>
+        <c:crossAx val="119614080"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="118958720"/>
+        <c:axId val="119614080"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1066,7 +1078,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="118957184"/>
+        <c:crossAx val="119612544"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -1105,15 +1117,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>5</xdr:col>
-      <xdr:colOff>30955</xdr:colOff>
-      <xdr:row>1</xdr:row>
-      <xdr:rowOff>52388</xdr:rowOff>
+      <xdr:colOff>16667</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>33338</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>14</xdr:col>
-      <xdr:colOff>333375</xdr:colOff>
-      <xdr:row>21</xdr:row>
-      <xdr:rowOff>95250</xdr:rowOff>
+      <xdr:colOff>319087</xdr:colOff>
+      <xdr:row>27</xdr:row>
+      <xdr:rowOff>76200</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -2060,10 +2072,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F28"/>
+  <dimension ref="A1:F35"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="200" zoomScaleNormal="200" workbookViewId="0">
-      <selection activeCell="D20" sqref="D20"/>
+    <sheetView tabSelected="1" topLeftCell="A19" zoomScale="200" zoomScaleNormal="200" workbookViewId="0">
+      <selection activeCell="D28" sqref="D28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -2278,88 +2290,137 @@
         <v>98.779693637604794</v>
       </c>
     </row>
-    <row r="17" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="C17" t="s">
+    <row r="16" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="B16">
+        <f>LINEST(B5:B15,A5:A15)</f>
+        <v>-6.8273320959649511E-2</v>
+      </c>
+      <c r="C16">
+        <f>LINEST(C5:C15,A5:A15)</f>
+        <v>-0.10649763016558562</v>
+      </c>
+      <c r="D16">
+        <f>LINEST(D5:D15,A5:A15)</f>
+        <v>-0.13287173851873768</v>
+      </c>
+    </row>
+    <row r="18" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B18" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="19" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B19" t="s">
+        <v>20</v>
+      </c>
+      <c r="C19">
+        <f>D16*60</f>
+        <v>-7.9723043111242609</v>
+      </c>
+    </row>
+    <row r="20" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B20" t="s">
+        <v>21</v>
+      </c>
+      <c r="C20">
+        <f>B16*60</f>
+        <v>-4.0963992575789705</v>
+      </c>
+    </row>
+    <row r="21" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B21" t="s">
+        <v>11</v>
+      </c>
+      <c r="C21">
+        <f>C16*60</f>
+        <v>-6.3898578099351377</v>
+      </c>
+    </row>
+    <row r="24" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B24" t="s">
+        <v>19</v>
+      </c>
+      <c r="C24" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="18" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="B18" t="s">
+    <row r="25" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B25" t="s">
         <v>9</v>
       </c>
-      <c r="C18" s="5">
+      <c r="C25" s="5">
         <f>0.0726*60</f>
         <v>4.3559999999999999</v>
       </c>
     </row>
-    <row r="19" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="B19" t="s">
+    <row r="26" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B26" t="s">
         <v>11</v>
       </c>
-      <c r="C19">
+      <c r="C26">
         <f>0.114*60</f>
         <v>6.84</v>
       </c>
     </row>
-    <row r="20" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="B20" t="s">
+    <row r="27" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B27" t="s">
         <v>12</v>
       </c>
-      <c r="C20">
+      <c r="C27">
         <f>0.1502*60</f>
         <v>9.0120000000000005</v>
       </c>
     </row>
-    <row r="23" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="B23" t="s">
+    <row r="30" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B30" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="24" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="E24">
+    <row r="31" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="E31">
         <v>256.70398554471103</v>
       </c>
     </row>
-    <row r="25" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="B25" t="s">
+    <row r="32" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B32" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="26" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="B26" t="s">
+    <row r="33" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B33" t="s">
         <v>15</v>
       </c>
-      <c r="C26" t="s">
+      <c r="C33" t="s">
         <v>16</v>
       </c>
-      <c r="E26" t="s">
+      <c r="E33" t="s">
         <v>17</v>
       </c>
-      <c r="F26" t="s">
+      <c r="F33" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="27" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="B27">
+    <row r="34" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B34">
         <v>15</v>
       </c>
-      <c r="C27">
+      <c r="C34">
         <v>96.5</v>
       </c>
-      <c r="E27">
+      <c r="E34">
         <f>(90-90.65)/(65-15)</f>
         <v>-1.3000000000000114E-2</v>
       </c>
-      <c r="F27">
-        <f>((0.013*E24)/100)*60</f>
+      <c r="F34">
+        <f>((0.013*E31)/100)*60</f>
         <v>2.002291087248746</v>
       </c>
     </row>
-    <row r="28" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="B28">
+    <row r="35" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B35">
         <v>65</v>
       </c>
-      <c r="C28">
+      <c r="C35">
         <v>90</v>
       </c>
     </row>

</xml_diff>